<commit_message>
started function to move data from excel sheet to mongo
</commit_message>
<xml_diff>
--- a/db_feed/new_template_v3.xlsx
+++ b/db_feed/new_template_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\volko\Desktop\Grover\DB\ofet-db\db_feed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C6D5D6-3F1E-42E8-91FF-7C0FBE0AF568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621409AC-A095-4F1F-9AEA-2F248091FF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{F8B411A1-6901-4B9B-966C-09D3D94CB0BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F8B411A1-6901-4B9B-966C-09D3D94CB0BB}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Data Origin" sheetId="9" r:id="rId1"/>
@@ -2271,6 +2271,16 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2291,16 +2301,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2619,7 +2619,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87527978-2A5B-6545-88F5-0DA220A53CEB}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView zoomScale="74" workbookViewId="0"/>
+    <sheetView topLeftCell="A2" zoomScale="74" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
@@ -2631,21 +2633,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="101" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="105" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="101"/>
+      <c r="B2" s="105"/>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" ht="15.6">
@@ -2935,8 +2937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6846DC66-F4E3-4EDA-AE74-F163B70AF782}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -3261,31 +3263,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.6" thickBot="1">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="101" t="s">
         <v>352</v>
       </c>
-      <c r="F1" s="104" t="s">
+      <c r="F1" s="108" t="s">
         <v>182</v>
       </c>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="106"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="110"/>
     </row>
     <row r="2" spans="1:9" ht="130.19999999999999" customHeight="1">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="106" t="s">
         <v>370</v>
       </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
       <c r="D2" s="3"/>
       <c r="I2" s="3"/>
     </row>
@@ -3734,7 +3736,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="18">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="103" t="s">
         <v>361</v>
       </c>
     </row>
@@ -4015,7 +4017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E323FD3-6C48-44BB-9F06-8E13A7AFDEDD}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -4032,31 +4034,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.6" thickBot="1">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="101" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="104" t="s">
+      <c r="F1" s="108" t="s">
         <v>182</v>
       </c>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="106"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="110"/>
     </row>
     <row r="2" spans="1:9" ht="127.5" customHeight="1">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="106" t="s">
         <v>370</v>
       </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="16.2" thickBot="1">
@@ -4430,34 +4432,34 @@
     <col min="7" max="7" width="34.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="111" customFormat="1" ht="21">
-      <c r="A1" s="108" t="s">
+    <row r="1" spans="1:7" s="104" customFormat="1" ht="21">
+      <c r="A1" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="111" t="s">
+      <c r="D1" s="104" t="s">
         <v>353</v>
       </c>
-      <c r="E1" s="111" t="s">
+      <c r="E1" s="104" t="s">
         <v>354</v>
       </c>
-      <c r="F1" s="111" t="s">
+      <c r="F1" s="104" t="s">
         <v>355</v>
       </c>
-      <c r="G1" s="111" t="s">
+      <c r="G1" s="104" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="111" t="s">
         <v>371</v>
       </c>
-      <c r="B2" s="107"/>
+      <c r="B2" s="111"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1"/>
     <row r="4" spans="1:7" s="8" customFormat="1" ht="16.95" customHeight="1">
@@ -4775,39 +4777,39 @@
     <col min="14" max="16384" width="8.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" s="111" customFormat="1" ht="21">
-      <c r="A1" s="111" t="s">
+    <row r="1" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" s="104" customFormat="1" ht="21">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="101" t="s">
         <v>353</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="101" t="s">
         <v>354</v>
       </c>
-      <c r="F1" s="108" t="s">
+      <c r="F1" s="101" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" s="8" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="102" t="s">
         <v>372</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" s="8" customFormat="1" ht="62.4" customHeight="1" thickBot="1">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="111" t="s">
         <v>373</v>
       </c>
-      <c r="B3" s="107"/>
-      <c r="C3" s="107"/>
+      <c r="B3" s="111"/>
+      <c r="C3" s="111"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
     </row>
@@ -7300,10 +7302,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="8" customFormat="1" ht="39.6" customHeight="1" thickBot="1">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="111" t="s">
         <v>375</v>
       </c>
-      <c r="B3" s="107"/>
+      <c r="B3" s="111"/>
     </row>
     <row r="4" spans="1:4" s="8" customFormat="1" ht="16.95" customHeight="1">
       <c r="A4" s="98" t="s">

</xml_diff>

<commit_message>
Ron's general update 12/6
new template to work with code, some helper functions, a file to populate certain collections with pre-determined solvents, update to main code
</commit_message>
<xml_diff>
--- a/db_feed/new_template_v3.xlsx
+++ b/db_feed/new_template_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\volko\Desktop\Grover\DB\ofet-db\db_feed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621409AC-A095-4F1F-9AEA-2F248091FF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC41B209-9BEA-4DBB-B4A1-42C9FFBB69BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F8B411A1-6901-4B9B-966C-09D3D94CB0BB}"/>
   </bookViews>
@@ -592,9 +592,6 @@
   </si>
   <si>
     <t>Eutactic</t>
-  </si>
-  <si>
-    <t>Polymer Semiconductor - wt% in solution</t>
   </si>
   <si>
     <t>The weight % (blend ratio) of the polymer semiconductor in solution</t>
@@ -1333,6 +1330,9 @@
   </si>
   <si>
     <t>Characterization File Type #</t>
+  </si>
+  <si>
+    <t>Semiconductor - wt% in solution</t>
   </si>
 </sst>
 </file>
@@ -2640,12 +2640,12 @@
         <v>1</v>
       </c>
       <c r="C1" s="101" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6">
       <c r="A2" s="105" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B2" s="105"/>
       <c r="C2" s="6"/>
@@ -2691,7 +2691,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.6">
       <c r="A9" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.6">
@@ -2705,12 +2705,12 @@
     </row>
     <row r="12" spans="1:3" ht="15.6">
       <c r="A12" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B13" s="11"/>
     </row>
@@ -2813,14 +2813,14 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="11" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" ht="15.6">
       <c r="A31" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="B34" s="31"/>
       <c r="C34" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2938,7 +2938,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -2961,13 +2961,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:6" ht="15.6">
       <c r="A2" s="14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1"/>
@@ -3011,7 +3011,7 @@
       </c>
       <c r="B7" s="83"/>
       <c r="D7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E7" s="58"/>
     </row>
@@ -3172,14 +3172,14 @@
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1">
       <c r="A25" s="87" t="s">
-        <v>177</v>
+        <v>376</v>
       </c>
       <c r="B25" s="89"/>
       <c r="C25" s="74" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E25" s="63"/>
     </row>
@@ -3247,7 +3247,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3273,10 +3273,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="101" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F1" s="108" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G1" s="109"/>
       <c r="H1" s="109"/>
@@ -3284,7 +3284,7 @@
     </row>
     <row r="2" spans="1:9" ht="130.19999999999999" customHeight="1">
       <c r="A2" s="106" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B2" s="107"/>
       <c r="C2" s="107"/>
@@ -3295,7 +3295,7 @@
       <c r="A3" s="15"/>
       <c r="D3" s="3"/>
       <c r="F3" s="45" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G3" s="45"/>
       <c r="H3" s="3"/>
@@ -3303,16 +3303,16 @@
     </row>
     <row r="4" spans="1:9" ht="16.2" thickBot="1">
       <c r="A4" s="39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="D4" s="41" t="s">
         <v>180</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>181</v>
       </c>
       <c r="F4" s="45"/>
       <c r="G4" s="45"/>
@@ -3321,65 +3321,65 @@
     </row>
     <row r="5" spans="1:9" ht="15.6">
       <c r="A5" s="49" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="84"/>
       <c r="C5" s="50"/>
       <c r="D5" s="51"/>
       <c r="F5" s="39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G5" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="H5" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="H5" s="40" t="s">
+      <c r="I5" s="41" t="s">
         <v>180</v>
-      </c>
-      <c r="I5" s="41" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="49" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B6" s="84"/>
       <c r="C6" s="50"/>
       <c r="D6" s="51"/>
       <c r="F6" s="36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G6" s="16"/>
       <c r="I6" s="37" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="49" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B7" s="84"/>
       <c r="C7" s="50" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D7" s="51"/>
       <c r="F7" s="36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G7" s="16"/>
       <c r="I7" s="37"/>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1">
       <c r="A8" s="49" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B8" s="84"/>
       <c r="C8" s="64" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D8" s="52"/>
       <c r="F8" s="44" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G8" s="42"/>
       <c r="H8" s="27"/>
@@ -3387,7 +3387,7 @@
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1">
       <c r="A9" s="44" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="65"/>
@@ -3396,45 +3396,45 @@
     </row>
     <row r="10" spans="1:9" ht="16.2" thickBot="1">
       <c r="F10" s="39" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G10" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="H10" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="I10" s="41" t="s">
         <v>180</v>
-      </c>
-      <c r="I10" s="41" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.6">
       <c r="A11" s="39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B11" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="D11" s="41" t="s">
         <v>180</v>
       </c>
-      <c r="D11" s="41" t="s">
-        <v>181</v>
-      </c>
       <c r="F11" s="36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G11" s="16"/>
       <c r="I11" s="37"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B12" s="34"/>
       <c r="D12" s="37"/>
       <c r="F12" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="27"/>
@@ -3442,13 +3442,13 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B13" s="34"/>
       <c r="C13" s="27"/>
       <c r="D13" s="37"/>
       <c r="F13" s="36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G13" s="16"/>
       <c r="H13" s="27"/>
@@ -3456,13 +3456,13 @@
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1">
       <c r="A14" s="36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B14" s="34"/>
       <c r="C14" s="27"/>
       <c r="D14" s="37"/>
       <c r="F14" s="44" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G14" s="99"/>
       <c r="H14" s="47"/>
@@ -3470,7 +3470,7 @@
     </row>
     <row r="15" spans="1:9" ht="16.2" thickBot="1">
       <c r="A15" s="46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B15" s="99"/>
       <c r="C15" s="47"/>
@@ -3479,10 +3479,10 @@
     </row>
     <row r="16" spans="1:9" ht="15.6">
       <c r="F16" s="39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H16" s="40" t="s">
         <v>81</v>
@@ -3493,7 +3493,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="F17" s="49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G17" s="48"/>
       <c r="H17" s="50"/>
@@ -3501,7 +3501,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="F18" s="49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G18" s="48"/>
       <c r="H18" s="50"/>
@@ -3509,7 +3509,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="F19" s="49" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G19" s="48"/>
       <c r="H19" s="50"/>
@@ -3517,7 +3517,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="F20" s="49" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="50"/>
@@ -3525,7 +3525,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="F21" s="49" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="50" t="s">
@@ -3538,7 +3538,7 @@
       <c r="C22" s="35"/>
       <c r="D22" s="35"/>
       <c r="F22" s="49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="27"/>
@@ -3546,7 +3546,7 @@
     </row>
     <row r="23" spans="1:9" ht="15" thickBot="1">
       <c r="F23" s="44" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G23" s="99"/>
       <c r="H23" s="47"/>
@@ -3558,28 +3558,28 @@
     </row>
     <row r="25" spans="1:9" ht="15.6">
       <c r="F25" s="39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G25" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="H25" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="H25" s="40" t="s">
+      <c r="I25" s="41" t="s">
         <v>180</v>
-      </c>
-      <c r="I25" s="41" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="F26" s="36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G26" s="16"/>
       <c r="I26" s="37"/>
     </row>
     <row r="27" spans="1:9">
       <c r="F27" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G27" s="16"/>
       <c r="H27" s="27"/>
@@ -3587,7 +3587,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="F28" s="36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="27"/>
@@ -3595,7 +3595,7 @@
     </row>
     <row r="29" spans="1:9" ht="16.2" thickBot="1">
       <c r="F29" s="46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G29" s="99"/>
       <c r="H29" s="47"/>
@@ -3609,21 +3609,21 @@
     </row>
     <row r="31" spans="1:9" ht="15.6">
       <c r="F31" s="39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G31" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="H31" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="H31" s="40" t="s">
+      <c r="I31" s="41" t="s">
         <v>180</v>
-      </c>
-      <c r="I31" s="41" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="F32" s="49" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G32" s="48"/>
       <c r="H32" s="50"/>
@@ -3631,7 +3631,7 @@
     </row>
     <row r="33" spans="6:9">
       <c r="F33" s="49" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G33" s="48"/>
       <c r="H33" s="50"/>
@@ -3639,27 +3639,27 @@
     </row>
     <row r="34" spans="6:9">
       <c r="F34" s="49" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G34" s="48"/>
       <c r="H34" s="38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I34" s="51"/>
     </row>
     <row r="35" spans="6:9">
       <c r="F35" s="49" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G35" s="16"/>
       <c r="H35" s="64" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I35" s="52"/>
     </row>
     <row r="36" spans="6:9" ht="15" thickBot="1">
       <c r="F36" s="44" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G36" s="99"/>
       <c r="H36" s="65"/>
@@ -3710,7 +3710,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -3737,17 +3737,17 @@
     </row>
     <row r="2" spans="1:4" ht="18">
       <c r="A2" s="103" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.2" thickBot="1">
       <c r="A3" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="54" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B4" s="55" t="s">
         <v>1</v>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="57" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="100"/>
@@ -3829,11 +3829,11 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="57" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B13" s="27"/>
       <c r="D13" s="59" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3855,7 +3855,7 @@
     </row>
     <row r="16" spans="1:4" s="1" customFormat="1">
       <c r="A16" s="57" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B16" s="34"/>
       <c r="C16" s="35" t="s">
@@ -3865,7 +3865,7 @@
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1">
       <c r="A17" s="57" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B17" s="34"/>
       <c r="C17" s="35" t="s">
@@ -3875,23 +3875,23 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="57" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B18" s="27"/>
       <c r="D18" s="58"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="57" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B19" s="27"/>
       <c r="D19" s="58" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="57" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B20" s="34"/>
       <c r="D20" s="58"/>
@@ -3905,7 +3905,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="57" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B22" s="34"/>
       <c r="C22" t="s">
@@ -3919,7 +3919,7 @@
       </c>
       <c r="B23" s="34"/>
       <c r="C23" s="27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D23" s="58"/>
     </row>
@@ -4017,7 +4017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E323FD3-6C48-44BB-9F06-8E13A7AFDEDD}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -4047,7 +4047,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="108" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G1" s="109"/>
       <c r="H1" s="109"/>
@@ -4055,7 +4055,7 @@
     </row>
     <row r="2" spans="1:9" ht="127.5" customHeight="1">
       <c r="A2" s="106" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B2" s="107"/>
       <c r="C2" s="107"/>
@@ -4064,7 +4064,7 @@
     <row r="3" spans="1:9" ht="16.2" thickBot="1">
       <c r="A3" s="79"/>
       <c r="F3" s="45" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G3" s="45"/>
       <c r="H3" s="3"/>
@@ -4072,10 +4072,10 @@
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1">
       <c r="A4" s="54" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C4" s="55" t="s">
         <v>2</v>
@@ -4084,40 +4084,40 @@
         <v>8</v>
       </c>
       <c r="F4" s="75" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="15.6">
       <c r="A5" s="36" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B5" s="26"/>
       <c r="D5" s="58" t="s">
         <v>49</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G5" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="H5" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="H5" s="40" t="s">
+      <c r="I5" s="41" t="s">
         <v>180</v>
-      </c>
-      <c r="I5" s="41" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="27"/>
       <c r="D6" s="58"/>
       <c r="F6" s="36" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G6" s="16"/>
       <c r="H6" t="s">
@@ -4134,11 +4134,11 @@
         <v>49</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G7" s="16"/>
       <c r="H7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I7" s="37"/>
     </row>
@@ -4150,12 +4150,12 @@
       <c r="C8" s="27"/>
       <c r="D8" s="58"/>
       <c r="F8" s="36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="27"/>
       <c r="I8" s="37" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1">
@@ -4164,11 +4164,11 @@
       </c>
       <c r="B9" s="42"/>
       <c r="C9" s="81" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D9" s="76"/>
       <c r="F9" s="44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G9" s="42"/>
       <c r="H9" s="74"/>
@@ -4180,10 +4180,10 @@
     <row r="11" spans="1:9" ht="16.2" thickBot="1">
       <c r="A11" s="9"/>
       <c r="F11" s="68" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G11" s="69" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H11" s="69" t="s">
         <v>81</v>
@@ -4194,19 +4194,19 @@
     </row>
     <row r="12" spans="1:9" ht="15.6">
       <c r="A12" s="39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B12" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="C12" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="D12" s="41" t="s">
         <v>180</v>
       </c>
-      <c r="D12" s="41" t="s">
-        <v>181</v>
-      </c>
       <c r="F12" s="49" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="64"/>
@@ -4214,7 +4214,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="36" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B13" s="16"/>
       <c r="C13" t="s">
@@ -4222,7 +4222,7 @@
       </c>
       <c r="D13" s="37"/>
       <c r="F13" s="49" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G13" s="16"/>
       <c r="H13" s="64"/>
@@ -4230,15 +4230,15 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="36" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D14" s="37"/>
       <c r="F14" s="49" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="64"/>
@@ -4246,31 +4246,31 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="27"/>
       <c r="D15" s="37" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F15" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="64" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I15" s="52"/>
     </row>
     <row r="16" spans="1:9" ht="15" thickBot="1">
       <c r="A16" s="44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B16" s="42"/>
       <c r="C16" s="74"/>
       <c r="D16" s="43"/>
       <c r="F16" s="49" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="64"/>
@@ -4278,12 +4278,12 @@
     </row>
     <row r="17" spans="6:9" ht="15" thickBot="1">
       <c r="F17" s="71" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G17" s="81"/>
       <c r="H17" s="73"/>
       <c r="I17" s="72" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18" spans="6:9" ht="16.2" thickBot="1">
@@ -4292,21 +4292,21 @@
     </row>
     <row r="19" spans="6:9" ht="15.6">
       <c r="F19" s="39" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G19" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="H19" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="H19" s="40" t="s">
+      <c r="I19" s="41" t="s">
         <v>180</v>
-      </c>
-      <c r="I19" s="41" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="20" spans="6:9" ht="15" thickBot="1">
       <c r="F20" s="44" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G20" s="42"/>
       <c r="H20" s="42"/>
@@ -4320,28 +4320,28 @@
     </row>
     <row r="22" spans="6:9" ht="15.6">
       <c r="F22" s="39" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G22" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="H22" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="H22" s="40" t="s">
+      <c r="I22" s="41" t="s">
         <v>180</v>
-      </c>
-      <c r="I22" s="41" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="23" spans="6:9">
       <c r="F23" s="36" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G23" s="27"/>
       <c r="I23" s="37"/>
     </row>
     <row r="24" spans="6:9">
       <c r="F24" s="36" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G24" s="67"/>
       <c r="H24" s="67"/>
@@ -4349,7 +4349,7 @@
     </row>
     <row r="25" spans="6:9">
       <c r="F25" s="36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G25" s="67"/>
       <c r="H25" s="67"/>
@@ -4357,7 +4357,7 @@
     </row>
     <row r="26" spans="6:9" ht="15" thickBot="1">
       <c r="F26" s="44" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G26" s="42"/>
       <c r="H26" s="42"/>
@@ -4419,7 +4419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74937810-402C-794A-86DB-3B61877792EA}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -4443,21 +4443,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="104" t="s">
+        <v>352</v>
+      </c>
+      <c r="E1" s="104" t="s">
         <v>353</v>
       </c>
-      <c r="E1" s="104" t="s">
+      <c r="F1" s="104" t="s">
         <v>354</v>
       </c>
-      <c r="F1" s="104" t="s">
-        <v>355</v>
-      </c>
       <c r="G1" s="104" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1">
       <c r="A2" s="111" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B2" s="111"/>
     </row>
@@ -4467,7 +4467,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>78</v>
@@ -4487,21 +4487,21 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="36" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B5" s="26"/>
       <c r="G5" s="58"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="36" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B6" s="26"/>
       <c r="G6" s="58"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="36" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B7" s="34"/>
       <c r="C7" t="s">
@@ -4511,28 +4511,28 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="36" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B8" s="34"/>
       <c r="G8" s="58"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="36" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B9" s="34"/>
       <c r="G9" s="58"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="36" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B10" s="34"/>
       <c r="G10" s="58"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="96" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B11" s="34"/>
       <c r="C11" t="s">
@@ -4544,7 +4544,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="36" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B12" s="34"/>
       <c r="C12" t="s">
@@ -4556,7 +4556,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="36" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B13" s="34"/>
       <c r="C13" t="s">
@@ -4568,7 +4568,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="96" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B14" s="34"/>
       <c r="C14" t="s">
@@ -4580,7 +4580,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="36" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B15" s="34"/>
       <c r="C15" t="s">
@@ -4592,7 +4592,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="36" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B16" s="34"/>
       <c r="C16" t="s">
@@ -4604,7 +4604,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="36" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B17" s="34"/>
       <c r="C17" t="s">
@@ -4616,7 +4616,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="36" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B18" s="34"/>
       <c r="C18" t="s">
@@ -4628,7 +4628,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="36" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B19" s="34"/>
       <c r="C19" t="s">
@@ -4640,7 +4640,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="36" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B20" s="34"/>
       <c r="D20" s="27"/>
@@ -4649,14 +4649,14 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="36" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B21" s="27"/>
       <c r="G21" s="58"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="36" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B22" s="34"/>
       <c r="C22" t="s">
@@ -4666,43 +4666,43 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="36" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B23" s="34"/>
       <c r="C23" t="s">
         <v>86</v>
       </c>
       <c r="G23" s="58" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="36" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B24" s="34"/>
       <c r="C24" t="s">
         <v>86</v>
       </c>
       <c r="G24" s="58" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="36" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B25" s="34"/>
       <c r="C25" t="s">
         <v>86</v>
       </c>
       <c r="G25" s="58" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1">
       <c r="A26" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B26" s="80"/>
       <c r="C26" s="74" t="s">
@@ -4788,25 +4788,25 @@
         <v>2</v>
       </c>
       <c r="D1" s="101" t="s">
+        <v>352</v>
+      </c>
+      <c r="E1" s="101" t="s">
         <v>353</v>
       </c>
-      <c r="E1" s="101" t="s">
-        <v>354</v>
-      </c>
       <c r="F1" s="101" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" s="8" customFormat="1" ht="60" customHeight="1">
       <c r="A2" s="102" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" s="8" customFormat="1" ht="62.4" customHeight="1" thickBot="1">
       <c r="A3" s="111" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B3" s="111"/>
       <c r="C3" s="111"/>
@@ -4815,13 +4815,13 @@
     </row>
     <row r="4" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" ht="15.6">
       <c r="A4" s="39" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>79</v>
@@ -4830,7 +4830,7 @@
         <v>80</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G4"/>
       <c r="H4"/>
@@ -6883,7 +6883,7 @@
     </row>
     <row r="5" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378">
       <c r="A5" s="36" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5"/>
@@ -6894,7 +6894,7 @@
     </row>
     <row r="6" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378">
       <c r="A6" s="36" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B6" s="34"/>
       <c r="C6"/>
@@ -6904,11 +6904,11 @@
     </row>
     <row r="7" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378">
       <c r="A7" s="36" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B7" s="34"/>
       <c r="C7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="34"/>
@@ -6916,7 +6916,7 @@
     </row>
     <row r="8" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" ht="15" thickBot="1">
       <c r="A8" s="44" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B8" s="80"/>
       <c r="C8" s="74"/>
@@ -6927,24 +6927,24 @@
     <row r="10" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" ht="15" thickBot="1"/>
     <row r="11" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" ht="15.6">
       <c r="A11" s="39" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D11" s="40"/>
       <c r="E11" s="40"/>
       <c r="F11" s="41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378">
       <c r="A12" s="36" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B12" s="34"/>
       <c r="C12"/>
@@ -6954,7 +6954,7 @@
     </row>
     <row r="13" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378">
       <c r="A13" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B13" s="34"/>
       <c r="C13"/>
@@ -6964,7 +6964,7 @@
     </row>
     <row r="14" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378">
       <c r="A14" s="36" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B14" s="34"/>
       <c r="C14"/>
@@ -6974,7 +6974,7 @@
     </row>
     <row r="15" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" ht="15" thickBot="1">
       <c r="A15" s="44" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B15" s="80"/>
       <c r="C15" s="74"/>
@@ -6985,23 +6985,23 @@
     <row r="17" spans="1:6" ht="15" thickBot="1"/>
     <row r="18" spans="1:6" ht="15.6">
       <c r="A18" s="39" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D18" s="40"/>
       <c r="E18" s="40"/>
       <c r="F18" s="41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="36" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B19" s="34"/>
       <c r="C19"/>
@@ -7011,7 +7011,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B20" s="34"/>
       <c r="C20" t="s">
@@ -7023,7 +7023,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="36" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B21" s="34"/>
       <c r="C21"/>
@@ -7033,7 +7033,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="36" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B22" s="34"/>
       <c r="C22" t="s">
@@ -7045,7 +7045,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="36" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B23" s="97"/>
       <c r="C23" t="s">
@@ -7057,11 +7057,11 @@
     </row>
     <row r="24" spans="1:6" ht="15" thickBot="1">
       <c r="A24" s="44" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B24" s="80"/>
       <c r="C24" s="74" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D24" s="81"/>
       <c r="E24" s="80"/>
@@ -7070,23 +7070,23 @@
     <row r="26" spans="1:6" ht="15" thickBot="1"/>
     <row r="27" spans="1:6" ht="15.6">
       <c r="A27" s="39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D27" s="40"/>
       <c r="E27" s="40"/>
       <c r="F27" s="41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="36" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B28" s="34"/>
       <c r="C28"/>
@@ -7096,11 +7096,11 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B29" s="34"/>
       <c r="C29" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D29" s="27"/>
       <c r="E29" s="34"/>
@@ -7108,7 +7108,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="36" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B30" s="34"/>
       <c r="C30"/>
@@ -7118,7 +7118,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="36" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B31" s="34"/>
       <c r="C31" t="s">
@@ -7130,7 +7130,7 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B32" s="34"/>
       <c r="C32"/>
@@ -7140,11 +7140,11 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B33" s="34"/>
       <c r="C33" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D33" s="27"/>
       <c r="E33" s="34"/>
@@ -7152,7 +7152,7 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="36" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B34" s="34"/>
       <c r="C34"/>
@@ -7162,7 +7162,7 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="36" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B35" s="34"/>
       <c r="C35" t="s">
@@ -7174,7 +7174,7 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="36" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B36" s="34"/>
       <c r="C36"/>
@@ -7184,7 +7184,7 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="36" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B37" s="97"/>
       <c r="C37" t="s">
@@ -7196,7 +7196,7 @@
     </row>
     <row r="38" spans="1:12" ht="15" thickBot="1">
       <c r="A38" s="44" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B38" s="80"/>
       <c r="C38" s="74"/>
@@ -7207,23 +7207,23 @@
     <row r="40" spans="1:12" ht="15" thickBot="1"/>
     <row r="41" spans="1:12" ht="15.6">
       <c r="A41" s="39" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B41" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D41" s="40"/>
       <c r="E41" s="40"/>
       <c r="F41" s="41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="36" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B42" s="34"/>
       <c r="C42"/>
@@ -7233,7 +7233,7 @@
     </row>
     <row r="43" spans="1:12" ht="15" thickBot="1">
       <c r="A43" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B43" s="80"/>
       <c r="C43" s="74" t="s">
@@ -7293,26 +7293,26 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" ht="16.8" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="8" customFormat="1" ht="39.6" customHeight="1" thickBot="1">
       <c r="A3" s="111" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B3" s="111"/>
     </row>
     <row r="4" spans="1:4" s="8" customFormat="1" ht="16.95" customHeight="1">
       <c r="A4" s="98" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C4" s="41" t="s">
         <v>53</v>
@@ -7320,42 +7320,42 @@
     </row>
     <row r="5" spans="1:4" s="8" customFormat="1" ht="16.95" customHeight="1">
       <c r="A5" s="36" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="58"/>
     </row>
     <row r="6" spans="1:4" s="8" customFormat="1" ht="16.95" customHeight="1">
       <c r="A6" s="36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B6" s="34"/>
       <c r="C6" s="58"/>
     </row>
     <row r="7" spans="1:4" s="8" customFormat="1" ht="17.25" customHeight="1">
       <c r="A7" s="36" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B7" s="34"/>
       <c r="C7" s="58"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B8" s="34"/>
       <c r="C8" s="58"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B9" s="34"/>
       <c r="C9" s="58"/>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1">
       <c r="A10" s="44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B10" s="80"/>
       <c r="C10" s="76"/>
@@ -63008,7 +63008,7 @@
         <v>25</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F25" s="21" t="s">
         <v>27</v>
@@ -63037,10 +63037,10 @@
         <v>127</v>
       </c>
       <c r="E27" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G27" t="s">
         <v>129</v>
@@ -63066,10 +63066,10 @@
         <v>128</v>
       </c>
       <c r="E28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G28" t="s">
         <v>116</v>
@@ -63089,7 +63089,7 @@
         <v>121</v>
       </c>
       <c r="F29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H29" t="s">
         <v>131</v>
@@ -63103,7 +63103,7 @@
         <v>122</v>
       </c>
       <c r="F30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H30" s="23" t="s">
         <v>132</v>
@@ -63195,32 +63195,32 @@
         <v>36</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D44" s="21" t="s">
         <v>50</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G44" s="21" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="F45" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B46" t="s">
         <v>145</v>
@@ -63232,21 +63232,21 @@
         <v>147</v>
       </c>
       <c r="E46" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G46" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H46" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B47" t="s">
         <v>146</v>
@@ -63261,13 +63261,13 @@
         <v>43</v>
       </c>
       <c r="F47" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G47" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H47" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -63275,21 +63275,21 @@
         <v>144</v>
       </c>
       <c r="C48" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D48" t="s">
         <v>149</v>
       </c>
       <c r="E48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C49" t="s">
         <v>149</v>
@@ -63297,7 +63297,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -63313,10 +63313,10 @@
         <v>82</v>
       </c>
       <c r="C53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D53" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -63327,10 +63327,10 @@
         <v>151</v>
       </c>
       <c r="C55" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D55" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -63341,10 +63341,10 @@
         <v>152</v>
       </c>
       <c r="C56" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D56" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -63352,10 +63352,10 @@
         <v>149</v>
       </c>
       <c r="B57" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C57" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>